<commit_message>
memperbaiki model untuk tahap 4
</commit_message>
<xml_diff>
--- a/public/format-kolom/Format Kolom Perusahaan.xlsx
+++ b/public/format-kolom/Format Kolom Perusahaan.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="format_perusahaan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="99">
   <si>
     <t>MEDAN</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>01-01-2024</t>
+  </si>
+  <si>
+    <t>kode_kegiatan</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC6"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,12 +1210,12 @@
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.42578125" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15" customWidth="1"/>
-    <col min="50" max="50" width="15" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15" customWidth="1"/>
+    <col min="51" max="51" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1274,88 +1283,91 @@
         <v>20</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
@@ -1431,8 +1443,8 @@
       <c r="Y2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="5">
-        <v>0</v>
+      <c r="Z2" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AA2" s="5">
         <v>0</v>
@@ -1440,8 +1452,8 @@
       <c r="AB2" s="5">
         <v>0</v>
       </c>
-      <c r="AC2" s="4" t="s">
-        <v>48</v>
+      <c r="AC2" s="5">
+        <v>0</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>48</v>
@@ -1449,8 +1461,8 @@
       <c r="AE2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="5">
-        <v>0</v>
+      <c r="AF2" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AG2" s="5">
         <v>0</v>
@@ -1458,8 +1470,8 @@
       <c r="AH2" s="5">
         <v>0</v>
       </c>
-      <c r="AI2" s="4" t="s">
-        <v>48</v>
+      <c r="AI2" s="5">
+        <v>0</v>
       </c>
       <c r="AJ2" s="4" t="s">
         <v>48</v>
@@ -1491,20 +1503,23 @@
       <c r="AS2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AT2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>48</v>
+      <c r="AT2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU2" s="5">
+        <v>0</v>
       </c>
       <c r="AV2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW2" s="5">
+      <c r="AW2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX2" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -1580,8 +1595,8 @@
       <c r="Y3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="5">
-        <v>0</v>
+      <c r="Z3" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AA3" s="5">
         <v>0</v>
@@ -1589,8 +1604,8 @@
       <c r="AB3" s="5">
         <v>0</v>
       </c>
-      <c r="AC3" s="4" t="s">
-        <v>48</v>
+      <c r="AC3" s="5">
+        <v>0</v>
       </c>
       <c r="AD3" s="4" t="s">
         <v>48</v>
@@ -1598,8 +1613,8 @@
       <c r="AE3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF3" s="5">
-        <v>0</v>
+      <c r="AF3" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AG3" s="5">
         <v>0</v>
@@ -1607,8 +1622,8 @@
       <c r="AH3" s="5">
         <v>0</v>
       </c>
-      <c r="AI3" s="4" t="s">
-        <v>48</v>
+      <c r="AI3" s="5">
+        <v>0</v>
       </c>
       <c r="AJ3" s="4" t="s">
         <v>48</v>
@@ -1640,20 +1655,23 @@
       <c r="AS3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AT3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>48</v>
+      <c r="AT3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>0</v>
       </c>
       <c r="AV3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="AW3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX3" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -1729,8 +1747,8 @@
       <c r="Y4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Z4" s="5">
-        <v>0</v>
+      <c r="Z4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AA4" s="5">
         <v>0</v>
@@ -1738,8 +1756,8 @@
       <c r="AB4" s="5">
         <v>0</v>
       </c>
-      <c r="AC4" s="4" t="s">
-        <v>48</v>
+      <c r="AC4" s="5">
+        <v>0</v>
       </c>
       <c r="AD4" s="4" t="s">
         <v>48</v>
@@ -1747,8 +1765,8 @@
       <c r="AE4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="5">
-        <v>0</v>
+      <c r="AF4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="AG4" s="5">
         <v>0</v>
@@ -1756,8 +1774,8 @@
       <c r="AH4" s="5">
         <v>0</v>
       </c>
-      <c r="AI4" s="4" t="s">
-        <v>48</v>
+      <c r="AI4" s="5">
+        <v>0</v>
       </c>
       <c r="AJ4" s="4" t="s">
         <v>48</v>
@@ -1789,20 +1807,23 @@
       <c r="AS4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AT4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>48</v>
+      <c r="AT4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>0</v>
       </c>
       <c r="AV4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW4" s="5">
+      <c r="AW4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX4" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
@@ -1869,99 +1890,102 @@
       <c r="V5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="X5" s="5">
         <v>78102</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="Z5" s="5">
         <v>85121</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="AA5" s="5">
         <v>2</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="AB5" s="5">
         <v>1</v>
       </c>
-      <c r="AB5" s="5">
-        <v>0</v>
-      </c>
       <c r="AC5" s="5">
-        <v>1995</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="5">
         <v>1995</v>
       </c>
-      <c r="AE5" s="8">
+      <c r="AE5" s="5">
+        <v>1995</v>
+      </c>
+      <c r="AF5" s="8">
         <v>220204360894</v>
       </c>
-      <c r="AF5" s="5">
+      <c r="AG5" s="5">
         <v>2</v>
       </c>
-      <c r="AG5" s="5">
+      <c r="AH5" s="5">
         <v>3</v>
       </c>
-      <c r="AH5" s="5">
+      <c r="AI5" s="5">
         <v>2</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL5" s="5">
+      <c r="AL5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM5" s="5">
         <v>138</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AN5" s="5">
         <v>32</v>
       </c>
-      <c r="AN5" s="5">
+      <c r="AO5" s="5">
         <v>3275</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AP5" s="5">
         <v>3275012</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AQ5" s="5">
+      <c r="AR5" s="5">
         <v>1</v>
       </c>
-      <c r="AR5" s="6">
+      <c r="AS5" s="6">
         <v>12699</v>
       </c>
-      <c r="AS5" s="5">
+      <c r="AT5" s="5">
         <v>138</v>
       </c>
-      <c r="AT5" s="5">
+      <c r="AU5" s="5">
         <v>1</v>
       </c>
-      <c r="AU5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="AV5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW5" s="5">
+      <c r="AW5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX5" s="5">
         <v>1</v>
       </c>
-      <c r="AX5" s="1"/>
-      <c r="BA5" t="s">
-        <v>48</v>
-      </c>
+      <c r="AY5" s="1"/>
       <c r="BB5" t="s">
         <v>48</v>
       </c>
-      <c r="BC5">
+      <c r="BC5" t="s">
+        <v>48</v>
+      </c>
+      <c r="BD5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
@@ -2028,44 +2052,44 @@
       <c r="V6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="X6" s="5">
         <v>47301</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="Y6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Z6" s="5">
         <v>33370</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="AA6" s="5">
         <v>2</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AB6" s="5">
         <v>1</v>
       </c>
-      <c r="AB6" s="5">
-        <v>0</v>
-      </c>
       <c r="AC6" s="5">
-        <v>1999</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="5">
         <v>1999</v>
       </c>
-      <c r="AE6" s="8">
+      <c r="AE6" s="5">
+        <v>1999</v>
+      </c>
+      <c r="AF6" s="8">
         <v>9120001821348</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AG6" s="5">
         <v>3</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AH6" s="5">
         <v>1</v>
       </c>
-      <c r="AH6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="4" t="s">
-        <v>48</v>
+      <c r="AI6" s="5">
+        <v>0</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>48</v>
@@ -2086,27 +2110,30 @@
         <v>48</v>
       </c>
       <c r="AP6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AQ6" s="5">
+      <c r="AR6" s="5">
         <v>1</v>
       </c>
-      <c r="AR6" s="6">
+      <c r="AS6" s="6">
         <v>30199</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AT6" s="5">
         <v>138</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AU6" s="5">
         <v>2</v>
       </c>
-      <c r="AU6" s="4" t="s">
+      <c r="AV6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AV6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AW6" s="5">
+      <c r="AW6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX6" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>